<commit_message>
Se modifican campos de seleccion, se agrega secuencia para devolver excel por Default
</commit_message>
<xml_diff>
--- a/fechas1.0.xlsx
+++ b/fechas1.0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msurrego\Desktop\BTHVTC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SICC\Documents\BthNotificacionVtc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4D58D9-A914-4D69-9C2C-816A62641C57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BD" sheetId="1" r:id="rId1"/>
@@ -23,17 +24,23 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BD!$A$1:$I$140</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FILTROXMES!$A$1:$F$18</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="355">
   <si>
     <t>N°</t>
   </si>
@@ -1097,100 +1104,13 @@
     <t>John German</t>
   </si>
   <si>
-    <t>30/1/2020</t>
-  </si>
-  <si>
-    <t>jueves</t>
-  </si>
-  <si>
-    <t>enero</t>
-  </si>
-  <si>
-    <t>enero 30</t>
-  </si>
-  <si>
-    <t>29/1/2020</t>
-  </si>
-  <si>
-    <t>miércoles</t>
-  </si>
-  <si>
-    <t>enero 29</t>
-  </si>
-  <si>
-    <t>domingo</t>
-  </si>
-  <si>
-    <t>enero 05</t>
-  </si>
-  <si>
-    <t>enero 01</t>
-  </si>
-  <si>
-    <t>19/1/2020</t>
-  </si>
-  <si>
-    <t>enero 19</t>
-  </si>
-  <si>
-    <t>enero 08</t>
-  </si>
-  <si>
-    <t>27/1/2020</t>
-  </si>
-  <si>
-    <t>lunes</t>
-  </si>
-  <si>
-    <t>enero 27</t>
-  </si>
-  <si>
-    <t>18/1/2020</t>
-  </si>
-  <si>
-    <t>sábado</t>
-  </si>
-  <si>
-    <t>enero 18</t>
-  </si>
-  <si>
-    <t>viernes</t>
-  </si>
-  <si>
-    <t>enero 03</t>
-  </si>
-  <si>
-    <t>14/1/2020</t>
-  </si>
-  <si>
-    <t>martes</t>
-  </si>
-  <si>
-    <t>enero 14</t>
-  </si>
-  <si>
-    <t>15/1/2020</t>
-  </si>
-  <si>
-    <t>enero 15</t>
-  </si>
-  <si>
-    <t>enero 04</t>
-  </si>
-  <si>
-    <t>enero 02</t>
-  </si>
-  <si>
-    <t>enero 06</t>
-  </si>
-  <si>
-    <t>enero 07</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="dddd"/>
     <numFmt numFmtId="165" formatCode="mmmm"/>
@@ -1429,9 +1349,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 13" xfId="1"/>
-    <cellStyle name="Normal 4" xfId="3"/>
-    <cellStyle name="Normal 6" xfId="2"/>
+    <cellStyle name="Normal 13" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 6" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1708,12 +1628,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J140"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.28515625" defaultRowHeight="27.75" customHeight="1"/>
   <cols>
@@ -6474,12 +6392,629 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J130"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="9" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="9"/>
+    <col min="9" max="9" width="13.85546875" style="9" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="15" customFormat="1" ht="36.75" customHeight="1">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="J6" s="9" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="F7" s="12"/>
+      <c r="J7" s="9" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="3:6">
+      <c r="C21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="C23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="C24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="3:6">
+      <c r="C25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="3:6">
+      <c r="C26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="3:6">
+      <c r="C27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="C28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="3:6">
+      <c r="C29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="3:6">
+      <c r="C30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="3:6">
+      <c r="C31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="3:6">
+      <c r="C32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+    </row>
+    <row r="33" spans="3:6">
+      <c r="C33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+    </row>
+    <row r="34" spans="3:6">
+      <c r="C34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+    </row>
+    <row r="35" spans="3:6">
+      <c r="C35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+    </row>
+    <row r="36" spans="3:6">
+      <c r="C36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+    </row>
+    <row r="37" spans="3:6">
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="3:6">
+      <c r="C38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="3:6">
+      <c r="C39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+    </row>
+    <row r="40" spans="3:6">
+      <c r="C40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+    </row>
+    <row r="41" spans="3:6">
+      <c r="C41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+    </row>
+    <row r="42" spans="3:6">
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+    </row>
+    <row r="43" spans="3:6">
+      <c r="C43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="3:6">
+      <c r="C44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" spans="3:6">
+      <c r="C45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+    </row>
+    <row r="46" spans="3:6">
+      <c r="C46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+    </row>
+    <row r="47" spans="3:6">
+      <c r="C47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+    </row>
+    <row r="48" spans="3:6">
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+    </row>
+    <row r="49" spans="3:6">
+      <c r="C49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+    </row>
+    <row r="50" spans="3:6">
+      <c r="C50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+    </row>
+    <row r="51" spans="3:6">
+      <c r="C51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+    </row>
+    <row r="52" spans="3:6">
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+    </row>
+    <row r="53" spans="3:6">
+      <c r="C53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+    </row>
+    <row r="54" spans="3:6">
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+    </row>
+    <row r="55" spans="3:6">
+      <c r="C55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+    </row>
+    <row r="56" spans="3:6">
+      <c r="C56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+    </row>
+    <row r="57" spans="3:6">
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+    </row>
+    <row r="58" spans="3:6">
+      <c r="C58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+    </row>
+    <row r="59" spans="3:6">
+      <c r="C59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+    </row>
+    <row r="60" spans="3:6">
+      <c r="C60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+    </row>
+    <row r="61" spans="3:6">
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+    </row>
+    <row r="62" spans="3:6">
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+    </row>
+    <row r="63" spans="3:6">
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+    </row>
+    <row r="64" spans="3:6">
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+    </row>
+    <row r="65" spans="3:6">
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+    </row>
+    <row r="66" spans="3:6">
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+    </row>
+    <row r="67" spans="3:6">
+      <c r="C67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+    </row>
+    <row r="68" spans="3:6">
+      <c r="C68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+    </row>
+    <row r="69" spans="3:6">
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+    </row>
+    <row r="70" spans="3:6">
+      <c r="C70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+    </row>
+    <row r="71" spans="3:6">
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+    </row>
+    <row r="72" spans="3:6">
+      <c r="C72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+    </row>
+    <row r="73" spans="3:6">
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+    </row>
+    <row r="74" spans="3:6">
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+    </row>
+    <row r="75" spans="3:6">
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+    </row>
+    <row r="76" spans="3:6">
+      <c r="C76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+    </row>
+    <row r="77" spans="3:6">
+      <c r="C77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+    </row>
+    <row r="78" spans="3:6">
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+    </row>
+    <row r="79" spans="3:6">
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+    </row>
+    <row r="80" spans="3:6">
+      <c r="C80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+    </row>
+    <row r="81" spans="3:6">
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+    </row>
+    <row r="82" spans="3:6">
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+    </row>
+    <row r="83" spans="3:6">
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+    </row>
+    <row r="84" spans="3:6">
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+    </row>
+    <row r="85" spans="3:6">
+      <c r="C85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+    </row>
+    <row r="86" spans="3:6">
+      <c r="C86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+    </row>
+    <row r="87" spans="3:6">
+      <c r="C87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+    </row>
+    <row r="88" spans="3:6">
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+    </row>
+    <row r="89" spans="3:6">
+      <c r="C89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
+    </row>
+    <row r="90" spans="3:6">
+      <c r="C90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+    </row>
+    <row r="91" spans="3:6">
+      <c r="C91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+    </row>
+    <row r="92" spans="3:6">
+      <c r="C92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+    </row>
+    <row r="93" spans="3:6">
+      <c r="C93" s="12"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="12"/>
+    </row>
+    <row r="94" spans="3:6">
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+    </row>
+    <row r="95" spans="3:6">
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+    </row>
+    <row r="96" spans="3:6">
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+    </row>
+    <row r="97" spans="5:6">
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+    </row>
+    <row r="98" spans="5:6">
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+    </row>
+    <row r="99" spans="5:6">
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+    </row>
+    <row r="100" spans="5:6">
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+    </row>
+    <row r="101" spans="5:6">
+      <c r="E101" s="12"/>
+      <c r="F101" s="12"/>
+    </row>
+    <row r="102" spans="5:6">
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+    </row>
+    <row r="103" spans="5:6">
+      <c r="E103" s="12"/>
+      <c r="F103" s="12"/>
+    </row>
+    <row r="104" spans="5:6">
+      <c r="E104" s="12"/>
+      <c r="F104" s="12"/>
+    </row>
+    <row r="105" spans="5:6">
+      <c r="E105" s="12"/>
+      <c r="F105" s="12"/>
+    </row>
+    <row r="106" spans="5:6">
+      <c r="E106" s="12"/>
+      <c r="F106" s="12"/>
+    </row>
+    <row r="107" spans="5:6">
+      <c r="E107" s="12"/>
+      <c r="F107" s="12"/>
+    </row>
+    <row r="108" spans="5:6">
+      <c r="E108" s="12"/>
+      <c r="F108" s="12"/>
+    </row>
+    <row r="109" spans="5:6">
+      <c r="E109" s="12"/>
+      <c r="F109" s="12"/>
+    </row>
+    <row r="110" spans="5:6">
+      <c r="E110" s="12"/>
+      <c r="F110" s="12"/>
+    </row>
+    <row r="111" spans="5:6">
+      <c r="E111" s="12"/>
+      <c r="F111" s="12"/>
+    </row>
+    <row r="112" spans="5:6">
+      <c r="E112" s="12"/>
+      <c r="F112" s="12"/>
+    </row>
+    <row r="113" spans="5:6">
+      <c r="E113" s="12"/>
+      <c r="F113" s="12"/>
+    </row>
+    <row r="114" spans="5:6">
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
+    </row>
+    <row r="115" spans="5:6">
+      <c r="E115" s="12"/>
+      <c r="F115" s="12"/>
+    </row>
+    <row r="116" spans="5:6">
+      <c r="E116" s="12"/>
+      <c r="F116" s="12"/>
+    </row>
+    <row r="117" spans="5:6">
+      <c r="E117" s="12"/>
+      <c r="F117" s="12"/>
+    </row>
+    <row r="118" spans="5:6">
+      <c r="E118" s="12"/>
+      <c r="F118" s="12"/>
+    </row>
+    <row r="119" spans="5:6">
+      <c r="E119" s="12"/>
+      <c r="F119" s="12"/>
+    </row>
+    <row r="120" spans="5:6">
+      <c r="E120" s="12"/>
+      <c r="F120" s="12"/>
+    </row>
+    <row r="121" spans="5:6">
+      <c r="E121" s="12"/>
+      <c r="F121" s="12"/>
+    </row>
+    <row r="122" spans="5:6">
+      <c r="E122" s="12"/>
+      <c r="F122" s="12"/>
+    </row>
+    <row r="123" spans="5:6">
+      <c r="E123" s="12"/>
+      <c r="F123" s="12"/>
+    </row>
+    <row r="124" spans="5:6">
+      <c r="E124" s="12"/>
+      <c r="F124" s="12"/>
+    </row>
+    <row r="125" spans="5:6">
+      <c r="E125" s="12"/>
+      <c r="F125" s="12"/>
+    </row>
+    <row r="126" spans="5:6">
+      <c r="E126" s="12"/>
+      <c r="F126" s="12"/>
+    </row>
+    <row r="127" spans="5:6">
+      <c r="E127" s="12"/>
+      <c r="F127" s="12"/>
+    </row>
+    <row r="128" spans="5:6">
+      <c r="E128" s="12"/>
+      <c r="F128" s="12"/>
+    </row>
+    <row r="129" spans="5:6">
+      <c r="E129" s="12"/>
+      <c r="F129" s="12"/>
+    </row>
+    <row r="130" spans="5:6">
+      <c r="E130" s="12"/>
+      <c r="F130" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6520,515 +7055,132 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="9">
-        <v>5</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>355</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>357</v>
-      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="9">
-        <v>6</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>358</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>360</v>
-      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="9">
-        <v>11</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="12">
-        <v>43952</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>361</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>362</v>
-      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="9">
-        <v>32</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="12">
-        <v>43831</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>363</v>
-      </c>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="9">
-        <v>41</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>361</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>365</v>
-      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="9">
-        <v>47</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="12">
-        <v>44044</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>366</v>
-      </c>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="9">
-        <v>62</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>367</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>368</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>369</v>
-      </c>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="9">
-        <v>83</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D9" s="12">
-        <v>44044</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>366</v>
-      </c>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="9">
-        <v>85</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>370</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>372</v>
-      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="9">
-        <v>90</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="D11" s="12">
-        <v>43891</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>373</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>374</v>
-      </c>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="9">
-        <v>93</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>375</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>376</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>377</v>
-      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="9">
-        <v>112</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>378</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>379</v>
-      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="9">
-        <v>132</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="D14" s="12">
-        <v>43922</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>380</v>
-      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="9">
-        <v>133</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>327</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>328</v>
-      </c>
-      <c r="D15" s="12">
-        <v>43862</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>355</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>381</v>
-      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="9">
-        <v>134</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>329</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="D16" s="12">
-        <v>43891</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>373</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="9">
-        <v>135</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>331</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="D17" s="12">
-        <v>43922</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="9">
-        <v>136</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="D18" s="12">
-        <v>43952</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="9">
-        <v>137</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="D19" s="12">
-        <v>43983</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>368</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="9">
-        <v>138</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="D20" s="12">
-        <v>44013</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>376</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="9">
-        <v>139</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="D21" s="12">
-        <v>44044</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="3:6">
+      <c r="C21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="3:6">
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="3:6">
       <c r="C23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="3:6">
       <c r="C24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="3:6">
       <c r="C25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="3:6">
       <c r="C26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="3:6">
       <c r="C27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="3:6">
       <c r="C28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="3:6">
       <c r="C29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="3:6">
       <c r="C30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="3:6">
       <c r="C31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="3:6">
       <c r="C32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
@@ -7463,17 +7615,20 @@
       <c r="F130" s="12"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F4">
+    <sortCondition ref="D2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7500,7 +7655,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="8" t="s">
@@ -7514,27 +7669,8 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="9">
-        <v>138</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="D2" s="12">
-        <v>44013</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>376</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>383</v>
-      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="12"/>
@@ -8093,20 +8229,16 @@
       <c r="F130" s="12"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F4">
-    <sortCondition ref="D2"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD21"/>
+      <selection activeCell="A2" sqref="A2:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -8711,12 +8843,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9319,612 +9451,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G130"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="9" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="9"/>
-    <col min="9" max="9" width="13.85546875" style="9" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>323</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="3:6">
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="3:6">
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="3:6">
-      <c r="C19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="3:6">
-      <c r="C20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="3:6">
-      <c r="C21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="3:6">
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="3:6">
-      <c r="C23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="3:6">
-      <c r="C24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="3:6">
-      <c r="C25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-    </row>
-    <row r="26" spans="3:6">
-      <c r="C26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="3:6">
-      <c r="C27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-    </row>
-    <row r="28" spans="3:6">
-      <c r="C28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-    </row>
-    <row r="29" spans="3:6">
-      <c r="C29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="3:6">
-      <c r="C30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="3:6">
-      <c r="C31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-    </row>
-    <row r="32" spans="3:6">
-      <c r="C32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-    </row>
-    <row r="33" spans="3:6">
-      <c r="C33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-    </row>
-    <row r="34" spans="3:6">
-      <c r="C34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-    </row>
-    <row r="35" spans="3:6">
-      <c r="C35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-    </row>
-    <row r="36" spans="3:6">
-      <c r="C36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-    </row>
-    <row r="37" spans="3:6">
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-    </row>
-    <row r="38" spans="3:6">
-      <c r="C38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-    </row>
-    <row r="39" spans="3:6">
-      <c r="C39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-    </row>
-    <row r="40" spans="3:6">
-      <c r="C40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-    </row>
-    <row r="41" spans="3:6">
-      <c r="C41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-    </row>
-    <row r="42" spans="3:6">
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-    </row>
-    <row r="43" spans="3:6">
-      <c r="C43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-    </row>
-    <row r="44" spans="3:6">
-      <c r="C44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-    </row>
-    <row r="45" spans="3:6">
-      <c r="C45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-    </row>
-    <row r="46" spans="3:6">
-      <c r="C46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-    </row>
-    <row r="47" spans="3:6">
-      <c r="C47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-    </row>
-    <row r="48" spans="3:6">
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-    </row>
-    <row r="49" spans="3:6">
-      <c r="C49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-    </row>
-    <row r="50" spans="3:6">
-      <c r="C50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-    </row>
-    <row r="51" spans="3:6">
-      <c r="C51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-    </row>
-    <row r="52" spans="3:6">
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-    </row>
-    <row r="53" spans="3:6">
-      <c r="C53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-    </row>
-    <row r="54" spans="3:6">
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-    </row>
-    <row r="55" spans="3:6">
-      <c r="C55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-    </row>
-    <row r="56" spans="3:6">
-      <c r="C56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-    </row>
-    <row r="57" spans="3:6">
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-    </row>
-    <row r="58" spans="3:6">
-      <c r="C58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-    </row>
-    <row r="59" spans="3:6">
-      <c r="C59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-    </row>
-    <row r="60" spans="3:6">
-      <c r="C60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-    </row>
-    <row r="61" spans="3:6">
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-    </row>
-    <row r="62" spans="3:6">
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-    </row>
-    <row r="63" spans="3:6">
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-    </row>
-    <row r="64" spans="3:6">
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-    </row>
-    <row r="65" spans="3:6">
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-    </row>
-    <row r="66" spans="3:6">
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-    </row>
-    <row r="67" spans="3:6">
-      <c r="C67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-    </row>
-    <row r="68" spans="3:6">
-      <c r="C68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-    </row>
-    <row r="69" spans="3:6">
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-    </row>
-    <row r="70" spans="3:6">
-      <c r="C70" s="12"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="12"/>
-    </row>
-    <row r="71" spans="3:6">
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-    </row>
-    <row r="72" spans="3:6">
-      <c r="C72" s="12"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-    </row>
-    <row r="73" spans="3:6">
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-    </row>
-    <row r="74" spans="3:6">
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
-    </row>
-    <row r="75" spans="3:6">
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
-    </row>
-    <row r="76" spans="3:6">
-      <c r="C76" s="12"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
-    </row>
-    <row r="77" spans="3:6">
-      <c r="C77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-    </row>
-    <row r="78" spans="3:6">
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-    </row>
-    <row r="79" spans="3:6">
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-    </row>
-    <row r="80" spans="3:6">
-      <c r="C80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-    </row>
-    <row r="81" spans="3:6">
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
-    </row>
-    <row r="82" spans="3:6">
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
-    </row>
-    <row r="83" spans="3:6">
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
-    </row>
-    <row r="84" spans="3:6">
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-    </row>
-    <row r="85" spans="3:6">
-      <c r="C85" s="12"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="12"/>
-    </row>
-    <row r="86" spans="3:6">
-      <c r="C86" s="12"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12"/>
-    </row>
-    <row r="87" spans="3:6">
-      <c r="C87" s="12"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="12"/>
-    </row>
-    <row r="88" spans="3:6">
-      <c r="E88" s="12"/>
-      <c r="F88" s="12"/>
-    </row>
-    <row r="89" spans="3:6">
-      <c r="C89" s="12"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="12"/>
-    </row>
-    <row r="90" spans="3:6">
-      <c r="C90" s="12"/>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12"/>
-    </row>
-    <row r="91" spans="3:6">
-      <c r="C91" s="12"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="12"/>
-    </row>
-    <row r="92" spans="3:6">
-      <c r="C92" s="12"/>
-      <c r="E92" s="12"/>
-      <c r="F92" s="12"/>
-    </row>
-    <row r="93" spans="3:6">
-      <c r="C93" s="12"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="12"/>
-    </row>
-    <row r="94" spans="3:6">
-      <c r="E94" s="12"/>
-      <c r="F94" s="12"/>
-    </row>
-    <row r="95" spans="3:6">
-      <c r="E95" s="12"/>
-      <c r="F95" s="12"/>
-    </row>
-    <row r="96" spans="3:6">
-      <c r="E96" s="12"/>
-      <c r="F96" s="12"/>
-    </row>
-    <row r="97" spans="5:6">
-      <c r="E97" s="12"/>
-      <c r="F97" s="12"/>
-    </row>
-    <row r="98" spans="5:6">
-      <c r="E98" s="12"/>
-      <c r="F98" s="12"/>
-    </row>
-    <row r="99" spans="5:6">
-      <c r="E99" s="12"/>
-      <c r="F99" s="12"/>
-    </row>
-    <row r="100" spans="5:6">
-      <c r="E100" s="12"/>
-      <c r="F100" s="12"/>
-    </row>
-    <row r="101" spans="5:6">
-      <c r="E101" s="12"/>
-      <c r="F101" s="12"/>
-    </row>
-    <row r="102" spans="5:6">
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
-    </row>
-    <row r="103" spans="5:6">
-      <c r="E103" s="12"/>
-      <c r="F103" s="12"/>
-    </row>
-    <row r="104" spans="5:6">
-      <c r="E104" s="12"/>
-      <c r="F104" s="12"/>
-    </row>
-    <row r="105" spans="5:6">
-      <c r="E105" s="12"/>
-      <c r="F105" s="12"/>
-    </row>
-    <row r="106" spans="5:6">
-      <c r="E106" s="12"/>
-      <c r="F106" s="12"/>
-    </row>
-    <row r="107" spans="5:6">
-      <c r="E107" s="12"/>
-      <c r="F107" s="12"/>
-    </row>
-    <row r="108" spans="5:6">
-      <c r="E108" s="12"/>
-      <c r="F108" s="12"/>
-    </row>
-    <row r="109" spans="5:6">
-      <c r="E109" s="12"/>
-      <c r="F109" s="12"/>
-    </row>
-    <row r="110" spans="5:6">
-      <c r="E110" s="12"/>
-      <c r="F110" s="12"/>
-    </row>
-    <row r="111" spans="5:6">
-      <c r="E111" s="12"/>
-      <c r="F111" s="12"/>
-    </row>
-    <row r="112" spans="5:6">
-      <c r="E112" s="12"/>
-      <c r="F112" s="12"/>
-    </row>
-    <row r="113" spans="5:6">
-      <c r="E113" s="12"/>
-      <c r="F113" s="12"/>
-    </row>
-    <row r="114" spans="5:6">
-      <c r="E114" s="12"/>
-      <c r="F114" s="12"/>
-    </row>
-    <row r="115" spans="5:6">
-      <c r="E115" s="12"/>
-      <c r="F115" s="12"/>
-    </row>
-    <row r="116" spans="5:6">
-      <c r="E116" s="12"/>
-      <c r="F116" s="12"/>
-    </row>
-    <row r="117" spans="5:6">
-      <c r="E117" s="12"/>
-      <c r="F117" s="12"/>
-    </row>
-    <row r="118" spans="5:6">
-      <c r="E118" s="12"/>
-      <c r="F118" s="12"/>
-    </row>
-    <row r="119" spans="5:6">
-      <c r="E119" s="12"/>
-      <c r="F119" s="12"/>
-    </row>
-    <row r="120" spans="5:6">
-      <c r="E120" s="12"/>
-      <c r="F120" s="12"/>
-    </row>
-    <row r="121" spans="5:6">
-      <c r="E121" s="12"/>
-      <c r="F121" s="12"/>
-    </row>
-    <row r="122" spans="5:6">
-      <c r="E122" s="12"/>
-      <c r="F122" s="12"/>
-    </row>
-    <row r="123" spans="5:6">
-      <c r="E123" s="12"/>
-      <c r="F123" s="12"/>
-    </row>
-    <row r="124" spans="5:6">
-      <c r="E124" s="12"/>
-      <c r="F124" s="12"/>
-    </row>
-    <row r="125" spans="5:6">
-      <c r="E125" s="12"/>
-      <c r="F125" s="12"/>
-    </row>
-    <row r="126" spans="5:6">
-      <c r="E126" s="12"/>
-      <c r="F126" s="12"/>
-    </row>
-    <row r="127" spans="5:6">
-      <c r="E127" s="12"/>
-      <c r="F127" s="12"/>
-    </row>
-    <row r="128" spans="5:6">
-      <c r="E128" s="12"/>
-      <c r="F128" s="12"/>
-    </row>
-    <row r="129" spans="5:6">
-      <c r="E129" s="12"/>
-      <c r="F129" s="12"/>
-    </row>
-    <row r="130" spans="5:6">
-      <c r="E130" s="12"/>
-      <c r="F130" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>